<commit_message>
modified:   CoinGecko_fetch.py 	new file:   coingecko_all_coins.xlsx 	modified:   coingecko_token_data.xlsx 	new file:   fetch_all_coins.py 	new file:   ~$coingecko_token_data.xlsx 	modified:   CoinGecko_fetch.py 	modified:   coingecko_all_coins.xlsx 	modified:   coingecko_token_data.xlsx 	deleted:    ~$coingecko_token_data.xlsx
</commit_message>
<xml_diff>
--- a/coingecko_token_data.xlsx
+++ b/coingecko_token_data.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>aave</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -467,820 +467,820 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4241199447</v>
+        <v>4862456468</v>
       </c>
       <c r="D2" t="n">
-        <v>15201727.01551733</v>
+        <v>15211264.30116868</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>ada</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ab-dao</t>
+          <t>cardano</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>30655930678</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>36362934086.75214</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>algo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>cardano</t>
+          <t>algorand</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>28256816358</v>
+        <v>2346196853</v>
       </c>
       <c r="D4" t="n">
-        <v>36172201725.55295</v>
+        <v>8706896055.327736</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>ape</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>arbitrum</t>
+          <t>apecoin</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2190826503</v>
+        <v>508773481</v>
       </c>
       <c r="D5" t="n">
-        <v>5150239630</v>
+        <v>799455492</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>apt</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>avalanche-2</t>
+          <t>aptos</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10042853349</v>
+        <v>3260757572</v>
       </c>
       <c r="D6" t="n">
-        <v>422276596.0335201</v>
+        <v>684332972.1450868</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BEAM</t>
+          <t>arb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>beam</t>
+          <t>arbitrum</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6769155</v>
+        <v>2441731436</v>
       </c>
       <c r="D7" t="n">
-        <v>184687550</v>
+        <v>5150239630</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BGB</t>
+          <t>asr</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>bitget-token</t>
+          <t>as-roma-fan-token</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5178722007</v>
+        <v>48687191</v>
       </c>
       <c r="D8" t="n">
-        <v>1139992036.1</v>
+        <v>7745096</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BONK</t>
+          <t>avax</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>bonk</t>
+          <t>avalanche-2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2239398870</v>
+        <v>10376800230</v>
       </c>
       <c r="D9" t="n">
-        <v>77419592329436.58</v>
+        <v>422276596.0335201</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CAKE</t>
+          <t>axs</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>pancakeswap-token</t>
+          <t>axie-infinity</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>980005585</v>
+        <v>420270732</v>
       </c>
       <c r="D10" t="n">
-        <v>344861864.1158483</v>
+        <v>166320222.4290032</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>bch</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>crypto-com-chain</t>
+          <t>bitcoin-cash</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4786787668</v>
+        <v>12009670414</v>
       </c>
       <c r="D11" t="n">
-        <v>32350617912.00131</v>
+        <v>19910696.77165078</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CRV</t>
+          <t>bgb</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>curve-dao-token</t>
+          <t>bitget-token</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1428047076</v>
+        <v>5055144911</v>
       </c>
       <c r="D12" t="n">
-        <v>1379658695</v>
+        <v>1139992035.978791</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>bonk</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>dogecoin</t>
+          <t>bonk</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>33510501031</v>
+        <v>2033551954</v>
       </c>
       <c r="D13" t="n">
-        <v>150243776383.7052</v>
+        <v>77419592329436.58</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>bnt</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>polkadot</t>
+          <t>bancor</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5901320780</v>
+        <v>94767919</v>
       </c>
       <c r="D14" t="n">
-        <v>1522267060</v>
+        <v>113836542.5460683</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>cro</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>multiversx</t>
+          <t>crypto-com-chain</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>5282395400</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>32384192415.06367</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ENS</t>
+          <t>crv</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ethereum-name-service</t>
+          <t>curve-dao-token</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>954040903</v>
+        <v>1385270155</v>
       </c>
       <c r="D16" t="n">
-        <v>33165585.05450796</v>
+        <v>1385810267</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FTM</t>
+          <t>cvx</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>fantom</t>
+          <t>convex-finance</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>372419702</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>81990703.72425415</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>FTN</t>
+          <t>doge</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>fasttoken</t>
+          <t>dogecoin</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1977511817</v>
+        <v>35452563636</v>
       </c>
       <c r="D18" t="n">
-        <v>431378783.4</v>
+        <v>150419716383.7052</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>gatechain-token</t>
+          <t>polkadot</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2087193937</v>
+        <v>6317026150</v>
       </c>
       <c r="D19" t="n">
-        <v>119444887.819009</v>
+        <v>1522267060</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>dydx</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>injective-protocol</t>
+          <t>dydx-chain</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1386770834</v>
+        <v>516350093</v>
       </c>
       <c r="D20" t="n">
-        <v>97727220.33</v>
+        <v>773348704.4859886</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>JASMY</t>
+          <t>ens</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>jasmycoin</t>
+          <t>ethereum-name-service</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>779619192</v>
+        <v>968898216</v>
       </c>
       <c r="D21" t="n">
-        <v>48419999999.3058</v>
+        <v>33165585.05450796</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>etc</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>kaspa</t>
+          <t>ethereum-classic</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2490794938</v>
+        <v>3619378642</v>
       </c>
       <c r="D22" t="n">
-        <v>26363807936.34678</v>
+        <v>153091726.9519364</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>KTA</t>
+          <t>fet</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>keeta</t>
+          <t>fetch-ai</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>484510736</v>
+        <v>1885862249</v>
       </c>
       <c r="D23" t="n">
-        <v>406082879.1212256</v>
+        <v>2604959126.672</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>fil</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>leo-token</t>
+          <t>filecoin</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>8265250995</v>
+        <v>1794763554</v>
       </c>
       <c r="D24" t="n">
-        <v>923042099.9</v>
+        <v>683864884</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>gala</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>chainlink</t>
+          <t>gala</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>12223281606</v>
+        <v>817148692</v>
       </c>
       <c r="D25" t="n">
-        <v>678099970.4527868</v>
+        <v>45613440228.21294</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>hbar</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>near</t>
+          <t>hedera-hashgraph</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3355974553</v>
+        <v>10984361437</v>
       </c>
       <c r="D26" t="n">
-        <v>1239916510</v>
+        <v>42392676005.9379</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>NFT</t>
+          <t>inj</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>apenft</t>
+          <t>injective-protocol</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>479100041</v>
+        <v>1448962586</v>
       </c>
       <c r="D27" t="n">
-        <v>990105682877398</v>
+        <v>97727220.33</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PENGU</t>
+          <t>jasmy</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>pudgy-penguins</t>
+          <t>jasmycoin</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2358824146</v>
+        <v>880853907</v>
       </c>
       <c r="D28" t="n">
-        <v>62860396090</v>
+        <v>48419999999.3058</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>kas</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>kaspa</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4859053849</v>
+        <v>2525455590</v>
       </c>
       <c r="D29" t="n">
-        <v>420690000000000</v>
+        <v>26363807936.34678</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>RENDER</t>
+          <t>kava</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>render-token</t>
+          <t>kava</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2059663890</v>
+        <v>425472961</v>
       </c>
       <c r="D30" t="n">
-        <v>518128769.0562826</v>
+        <v>1082853140</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SATS</t>
+          <t>ldo</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>sats-ordinals</t>
+          <t>lido-dao</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>87249198</v>
+        <v>1391369525</v>
       </c>
       <c r="D31" t="n">
-        <v>2100000000000000</v>
+        <v>895888862.5921584</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>shiba-inu</t>
+          <t>leo-2</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>7700717120</v>
+        <v>1508205</v>
       </c>
       <c r="D32" t="n">
-        <v>589246227519549.4</v>
+        <v>999890689.477294</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SKY</t>
+          <t>link</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>sky</t>
+          <t>chainlink</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1836141238</v>
+        <v>16087346903</v>
       </c>
       <c r="D33" t="n">
-        <v>21254542614.79155</v>
+        <v>678099970.4527868</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SUI</t>
+          <t>mana</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>sui</t>
+          <t>decentraland</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>13304636249</v>
+        <v>590322260</v>
       </c>
       <c r="D34" t="n">
-        <v>3455015252.817221</v>
+        <v>1919188956.588888</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SUN</t>
+          <t>near</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>sun-token</t>
+          <t>near</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>418807859</v>
+        <v>3499959779</v>
       </c>
       <c r="D35" t="n">
-        <v>19153216630.86329</v>
+        <v>1246897382</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SYRUP</t>
+          <t>ondo</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>maple-finance</t>
+          <t>ondo-finance</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>3320027594</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>3159107529</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>paxg</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>bittensor</t>
+          <t>pax-gold</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3587234791</v>
+        <v>949628420</v>
       </c>
       <c r="D37" t="n">
-        <v>9512306</v>
+        <v>284182.589</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>pendle</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>the-open-network</t>
+          <t>pendle</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>8307834941</v>
+        <v>912572593</v>
       </c>
       <c r="D38" t="n">
-        <v>2416091720.841465</v>
+        <v>167445463.8527003</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>tron</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>30970238493</v>
+        <v>5112432040</v>
       </c>
       <c r="D39" t="n">
-        <v>94720386625.43184</v>
+        <v>420690000000000</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>USELESS</t>
+          <t>sand</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>useless-3</t>
+          <t>the-sandbox</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>306184130</v>
+        <v>734572750</v>
       </c>
       <c r="D40" t="n">
-        <v>999940362.02</v>
+        <v>2445857126.223322</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>WAL</t>
+          <t>sei</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>walrus-2</t>
+          <t>sei-network</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>590897745</v>
+        <v>1877534811</v>
       </c>
       <c r="D41" t="n">
-        <v>1380833333</v>
+        <v>5781805555</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>WEMIX</t>
+          <t>shib</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>wemix-token</t>
+          <t>shiba-inu</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>424699333</v>
+        <v>7977124285</v>
       </c>
       <c r="D42" t="n">
-        <v>453724894.1429949</v>
+        <v>589246036829115.8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>sui</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>sui</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>13551437650</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>3511924479.569998</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>uni</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>stellar</t>
+          <t>uniswap</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>13236853917</v>
+        <v>6901381154</v>
       </c>
       <c r="D44" t="n">
-        <v>31217692899.09495</v>
+        <v>600483073.71</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>xlm</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>monero</t>
+          <t>stellar</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5822598369</v>
+        <v>13877106318</v>
       </c>
       <c r="D45" t="n">
-        <v>18446744.07370955</v>
+        <v>31298889990.9876</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>xmr</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ripple</t>
+          <t>monero</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>185912748317</v>
+        <v>4556243690</v>
       </c>
       <c r="D46" t="n">
-        <v>59239646627</v>
+        <v>18446744.07370955</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ZIG</t>
+          <t>xrp</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>zignaly</t>
+          <t>ripple</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>143162008</v>
+        <v>190750152823</v>
       </c>
       <c r="D47" t="n">
-        <v>1408940795.239652</v>
+        <v>59308385925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   CoinGecko_fetch.py 	modified:   coingecko_token_data.xlsx 	new file:   coingecko_top200_market_cap.xlsx 	modified:   fetch_all_coins.py 	new file:   volume_spike_24h.py
</commit_message>
<xml_diff>
--- a/coingecko_token_data.xlsx
+++ b/coingecko_token_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,468 +458,986 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>aave</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>aave</t>
-        </is>
-      </c>
       <c r="C2" t="n">
-        <v>4295706147</v>
+        <v>3625994846</v>
       </c>
       <c r="D2" t="n">
-        <v>15250277.18133271</v>
+        <v>15254085.97531263</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ankr</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ankr</t>
+          <t>cardano</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>137658290</v>
+        <v>23948249853</v>
       </c>
       <c r="D3" t="n">
-        <v>10000000000</v>
+        <v>36552429492.24524</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ape</t>
+          <t>AERO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>apecoin</t>
+          <t>aerodrome-finance</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>509234979</v>
+        <v>773149461</v>
       </c>
       <c r="D4" t="n">
-        <v>908664773</v>
+        <v>905398303.0906532</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>arb</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>arbitrum</t>
+          <t>algorand</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2327711870</v>
+        <v>1676858916</v>
       </c>
       <c r="D5" t="n">
-        <v>5403630609</v>
+        <v>8809933221.077435</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>avax</t>
+          <t>ANKR</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>avalanche-2</t>
+          <t>ankr</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12667913297</v>
+        <v>105073279</v>
       </c>
       <c r="D6" t="n">
-        <v>422276596.0335201</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>bch</t>
+          <t>APE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>bitcoin-cash</t>
+          <t>apecoin</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11827627411</v>
+        <v>343400134</v>
       </c>
       <c r="D7" t="n">
-        <v>19934340.52165078</v>
+        <v>908664773</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>bonk</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>bonk</t>
+          <t>aptos</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1530938148</v>
+        <v>2681544197</v>
       </c>
       <c r="D8" t="n">
-        <v>77419592329436.58</v>
+        <v>705029414.9554992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>c98</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>coin98</t>
+          <t>arbitrum</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>65551638</v>
+        <v>1716846496</v>
       </c>
       <c r="D9" t="n">
-        <v>999999711</v>
+        <v>5403630609</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>chz</t>
+          <t>ASR</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>chiliz</t>
+          <t>as-roma-fan-token</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>444747193</v>
+        <v>13038625</v>
       </c>
       <c r="D10" t="n">
-        <v>10022747118</v>
+        <v>7914126</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>crv</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>curve-dao-token</t>
+          <t>avalanche-2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1087448559</v>
+        <v>9699447024</v>
       </c>
       <c r="D11" t="n">
-        <v>1408953862</v>
+        <v>426272092.6113223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>cvx</t>
+          <t>AXS</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>convex-finance</t>
+          <t>axie-infinity</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>301509757</v>
+        <v>264634994</v>
       </c>
       <c r="D12" t="n">
-        <v>81990703.72425415</v>
+        <v>166529088.7561391</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>dydx</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>dydx-chain</t>
+          <t>bitcoin-cash</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>483297603</v>
+        <v>10318213600</v>
       </c>
       <c r="D13" t="n">
-        <v>786925345.5275061</v>
+        <v>19937587.39665078</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ens</t>
+          <t>BGB</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ethereum-name-service</t>
+          <t>bitget-token</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>701269825</v>
+        <v>3374528257</v>
       </c>
       <c r="D14" t="n">
-        <v>33165585.05450796</v>
+        <v>699992035.9787906</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>fet</t>
+          <t>BNT</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>fetch-ai</t>
+          <t>bancor</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1506449116</v>
+        <v>65483238</v>
       </c>
       <c r="D15" t="n">
-        <v>2604959126.672</v>
+        <v>111811528.573549</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>fil</t>
+          <t>BONK</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>filecoin</t>
+          <t>bonk</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1590315002</v>
+        <v>1096019026</v>
       </c>
       <c r="D16" t="n">
-        <v>693831865</v>
+        <v>77419592329436.58</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>floki</t>
+          <t>C98</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>floki</t>
+          <t>coin98</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>997306843</v>
+        <v>37123494</v>
       </c>
       <c r="D17" t="n">
-        <v>9659271645437</v>
+        <v>999999711</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>gala</t>
+          <t>CHZ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>gala</t>
+          <t>chiliz</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>716472377</v>
+        <v>327654250</v>
       </c>
       <c r="D18" t="n">
-        <v>46096805694.25091</v>
+        <v>10036224564</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>inj</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>injective-protocol</t>
+          <t>crypto-com-chain</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1252313585</v>
+        <v>5538767545</v>
       </c>
       <c r="D19" t="n">
-        <v>97727220.33</v>
+        <v>34869518367.82087</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>jasmy</t>
+          <t>CRV</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>jasmycoin</t>
+          <t>curve-dao-token</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>617337918</v>
+        <v>717630817</v>
       </c>
       <c r="D20" t="n">
-        <v>48419999999.3058</v>
+        <v>1411497555</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>mana</t>
+          <t>CVX</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>decentraland</t>
+          <t>convex-finance</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>640101254</v>
+        <v>191006504</v>
       </c>
       <c r="D21" t="n">
-        <v>1919164175.113888</v>
+        <v>81990703.72425415</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>near</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>near</t>
+          <t>dogecoin</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3629385752</v>
+        <v>29192429099</v>
       </c>
       <c r="D22" t="n">
-        <v>1249836992</v>
+        <v>151282016383.7052</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>polkadot</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4043881786</v>
+        <v>4771449085</v>
       </c>
       <c r="D23" t="n">
-        <v>420690000000000</v>
+        <v>1522267060</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>reef</t>
+          <t>DYDX</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>reef</t>
+          <t>dydx-chain</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>13065958</v>
+        <v>289450399</v>
       </c>
       <c r="D24" t="n">
-        <v>43966651824.25184</v>
+        <v>790379768.5275061</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>sand</t>
+          <t>ENS</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>the-sandbox</t>
+          <t>ethereum-name-service</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>677115554</v>
+        <v>519087472</v>
       </c>
       <c r="D25" t="n">
-        <v>2445857126.223322</v>
+        <v>33165585.05450796</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>sxp</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>swipe</t>
+          <t>ethereum-classic</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>104961339</v>
+        <v>2351212097</v>
       </c>
       <c r="D26" t="n">
-        <v>655170869.9034001</v>
+        <v>153871275.4978417</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>zrx</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>fetch-ai</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1023735240</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2604959126.672</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>FIL</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>filecoin</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1151980724</v>
+      </c>
+      <c r="D28" t="n">
+        <v>702332204</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>FLOKI</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>floki</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>672269606</v>
+      </c>
+      <c r="D29" t="n">
+        <v>9658943166302</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>GALA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>gala</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>504654037</v>
+      </c>
+      <c r="D30" t="n">
+        <v>46174358862.70763</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>HBAR</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>hedera-hashgraph</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>7374829439</v>
+      </c>
+      <c r="D31" t="n">
+        <v>42401692972.15297</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>INJ</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>injective-protocol</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>866876896</v>
+      </c>
+      <c r="D32" t="n">
+        <v>97727220.33</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>JASMY</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>jasmycoin</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>497532189</v>
+      </c>
+      <c r="D33" t="n">
+        <v>48419999999.3058</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>KAVA</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>kava</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>205899232</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1082853067</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>LDO</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>lido-dao</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>758845641</v>
+      </c>
+      <c r="D35" t="n">
+        <v>895801548.0664213</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>chainlink</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>12469618744</v>
+      </c>
+      <c r="D36" t="n">
+        <v>696849970.4525868</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>MANA</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>decentraland</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>469654718</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1919162174.188888</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>near</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>2957985575</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1249836992</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ONDO</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ondo-finance</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2371669928</v>
+      </c>
+      <c r="D39" t="n">
+        <v>3159107529</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>PAXG</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>pax-gold</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1221821606</v>
+      </c>
+      <c r="D40" t="n">
+        <v>306671.574</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>PENDLE</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>pendle</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>613248120</v>
+      </c>
+      <c r="D41" t="n">
+        <v>169918520.4159158</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>pepe</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>2960693032</v>
+      </c>
+      <c r="D42" t="n">
+        <v>420690000000000</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>REEF</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>reef</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>10868337</v>
+      </c>
+      <c r="D43" t="n">
+        <v>43892928960.80034</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>RENDER</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>render-token</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1275864885</v>
+      </c>
+      <c r="D44" t="n">
+        <v>518584616.1640741</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>RTXWETH</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SAND</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>the-sandbox</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>494797878</v>
+      </c>
+      <c r="D46" t="n">
+        <v>2445857126.223322</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SEI</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>sei-network</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>1332291167</v>
+      </c>
+      <c r="D47" t="n">
+        <v>6127777777</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SHIB</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>shiba-inu</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>6089410153</v>
+      </c>
+      <c r="D48" t="n">
+        <v>589245755895143.9</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>sui</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>9674702901</v>
+      </c>
+      <c r="D49" t="n">
+        <v>3625742933.075554</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SXP</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>swipe</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>80434920</v>
+      </c>
+      <c r="D50" t="n">
+        <v>658574689.6964231</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TAO</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>bittensor</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>2930161490</v>
+      </c>
+      <c r="D51" t="n">
+        <v>9597491</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>uniswap</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>3643062238</v>
+      </c>
+      <c r="D52" t="n">
+        <v>600483073.71</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>VET</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>vechain</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1490852807</v>
+      </c>
+      <c r="D53" t="n">
+        <v>85985041177</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>XLM</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>stellar</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>10547023896</v>
+      </c>
+      <c r="D54" t="n">
+        <v>32018846809.25486</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>XMR</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>monero</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>5611020631</v>
+      </c>
+      <c r="D55" t="n">
+        <v>18446744.07370955</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ZRX</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>0x</t>
         </is>
       </c>
-      <c r="C27" t="n">
-        <v>210903881</v>
-      </c>
-      <c r="D27" t="n">
+      <c r="C56" t="n">
+        <v>169028497</v>
+      </c>
+      <c r="D56" t="n">
         <v>848396562.906836</v>
       </c>
     </row>

</xml_diff>